<commit_message>
func!: add version 'v250811' of main functionality to display song lyrics.
Second version of main functionality in folder 'v250811'.
</commit_message>
<xml_diff>
--- a/rsrcs/_support_files/song-lemon_demon-fine-timestamps.xlsx
+++ b/rsrcs/_support_files/song-lemon_demon-fine-timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arbela1t0\Downloads\programming_and_coding-dev_containers\project-python-song_lyrics_terminal_console_display-d250810\rsrcs\_support_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B25705A-7113-4D9C-9D61-47025DB9E436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8807D07-3AE8-4C4C-952C-68A3A3FBF5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,9 +520,6 @@
     <t>[00:00.00][. . .]</t>
   </si>
   <si>
-    <t>[-00:10.00][positive_offset]</t>
-  </si>
-  <si>
     <t>import_adjusted_lrc</t>
   </si>
   <si>
@@ -569,6 +566,9 @@
   </si>
   <si>
     <t>line_end_delay</t>
+  </si>
+  <si>
+    <t>[-00:07.00][positive_offset]</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07CDD681-A3E3-4157-8C3C-72B6F4057F72}">
   <dimension ref="A1:AM82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AM19" sqref="AM19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="2" x14ac:dyDescent="0.3"/>
@@ -1474,19 +1474,19 @@
       <c r="AE4" s="29"/>
       <c r="AF4" s="29"/>
       <c r="AG4" s="64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AH4" s="33" t="s">
         <v>137</v>
       </c>
       <c r="AI4" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AJ4" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AK4" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AL4" s="67" t="s">
         <v>137</v>
@@ -1540,19 +1540,19 @@
       <c r="AE5" s="29"/>
       <c r="AF5" s="29"/>
       <c r="AG5" s="65" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AH5" s="33" t="s">
         <v>137</v>
       </c>
       <c r="AI5" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="AJ5" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="AJ5" s="33" t="s">
-        <v>169</v>
-      </c>
       <c r="AK5" s="33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AL5" s="67" t="s">
         <v>137</v>
@@ -1587,13 +1587,13 @@
       <c r="AG6" s="65"/>
       <c r="AH6" s="33"/>
       <c r="AI6" s="33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AJ6" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AK6" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AL6" s="67" t="s">
         <v>137</v>
@@ -1661,7 +1661,7 @@
       <c r="C9" s="52"/>
       <c r="D9" s="52"/>
       <c r="E9" s="68" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F9" s="39" t="s">
         <v>81</v>
@@ -1726,13 +1726,13 @@
       <c r="AH9" s="52"/>
       <c r="AI9" s="52"/>
       <c r="AJ9" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="AK9" s="70" t="s">
         <v>175</v>
       </c>
-      <c r="AK9" s="70" t="s">
+      <c r="AL9" s="69" t="s">
         <v>176</v>
-      </c>
-      <c r="AL9" s="69" t="s">
-        <v>177</v>
       </c>
       <c r="AM9" s="53"/>
     </row>
@@ -1741,7 +1741,7 @@
         <v>155</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>75</v>
@@ -1846,7 +1846,7 @@
         <v>108</v>
       </c>
       <c r="AK10" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AL10" s="21" t="s">
         <v>109</v>
@@ -2488,11 +2488,11 @@
         <v>5</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="C15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-00:10.00</v>
+        <v>-00:07.00</v>
       </c>
       <c r="D15" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2504,11 +2504,11 @@
       </c>
       <c r="F15" s="58">
         <f t="shared" si="35"/>
-        <v>-1.1574074074074075E-4</v>
+        <v>-8.1018518518518516E-5</v>
       </c>
       <c r="G15" s="9">
         <f t="shared" si="4"/>
-        <v>-1.1574074074074075E-4</v>
+        <v>-8.1018518518518516E-5</v>
       </c>
       <c r="H15" s="11" t="e">
         <f t="shared" si="5"/>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="O15" s="14">
         <f t="shared" si="12"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P15" s="11" t="e">
         <f t="shared" si="13"/>
@@ -2548,7 +2548,7 @@
       </c>
       <c r="Q15" s="9">
         <f t="shared" si="14"/>
-        <v>-1.1574074074074075E-4</v>
+        <v>-8.1018518518518516E-5</v>
       </c>
       <c r="R15" s="15" t="e">
         <f t="shared" si="15"/>
@@ -2560,7 +2560,7 @@
       </c>
       <c r="T15" s="9">
         <f t="shared" si="17"/>
-        <v>-2.7777777777777779E-3</v>
+        <v>-1.9444444444444444E-3</v>
       </c>
       <c r="U15" s="15" t="e">
         <f t="shared" si="18"/>
@@ -2572,7 +2572,7 @@
       </c>
       <c r="W15" s="9">
         <f t="shared" si="20"/>
-        <v>-0.16666666666666669</v>
+        <v>-0.11666666666666667</v>
       </c>
       <c r="X15" s="15" t="e">
         <f t="shared" si="21"/>
@@ -2584,7 +2584,7 @@
       </c>
       <c r="Z15" s="8">
         <f t="shared" si="23"/>
-        <v>-10.000000000000002</v>
+        <v>-7</v>
       </c>
       <c r="AA15" s="16" t="e">
         <f t="shared" si="24"/>
@@ -2596,7 +2596,7 @@
       </c>
       <c r="AC15" s="7">
         <f t="shared" si="25"/>
-        <v>-10000.000000000002</v>
+        <v>-7000</v>
       </c>
       <c r="AD15" s="17" t="e">
         <f t="shared" si="26"/>
@@ -2612,11 +2612,11 @@
       </c>
       <c r="AG15" s="63">
         <f>+F16-F15</f>
-        <v>1.1574074074074075E-4</v>
+        <v>8.1018518518518516E-5</v>
       </c>
       <c r="AH15" s="8">
         <f t="shared" si="29"/>
-        <v>10.000000000000002</v>
+        <v>7</v>
       </c>
       <c r="AI15" s="6">
         <f t="shared" si="30"/>
@@ -2628,15 +2628,15 @@
       </c>
       <c r="AK15" s="55">
         <f t="shared" si="32"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AL15" s="47">
         <f t="shared" si="33"/>
-        <v>1.2</v>
+        <v>0.4</v>
       </c>
       <c r="AM15" s="4" t="str">
         <f>+_xlfn.CONCAT(CHAR(34),$E15,CHAR(34),", ",AJ15,", ",AK15,", ",AL15)</f>
-        <v>"[delay]", 0.2, 4, 1.2</v>
+        <v>"[delay]", 0.2, 3, 0.4</v>
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
@@ -2952,7 +2952,7 @@
     <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" s="54"/>
       <c r="B18" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" s="4" t="str">
         <f t="shared" si="0"/>
@@ -11855,7 +11855,7 @@
         <v>Everything works out nice in the end</v>
       </c>
       <c r="E75" s="4" t="str">
-        <f t="shared" ref="E75:E106" si="48">+IF(OR(D75="",D75="[. . .]"),$C$5,IF(D75="[positive_offset]",$C$6,D75))</f>
+        <f t="shared" ref="E75:E81" si="48">+IF(OR(D75="",D75="[. . .]"),$C$5,IF(D75="[positive_offset]",$C$6,D75))</f>
         <v>Everything works out nice in the end</v>
       </c>
       <c r="F75" s="58">
@@ -11983,7 +11983,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="AK75" s="55">
-        <f t="shared" ref="AK75:AK106" si="56">+IF(OR($E75=$C$5,$E75=$C$6),ROUNDDOWN(AH75/(AI75*AJ75),0),1)</f>
+        <f t="shared" ref="AK75:AK81" si="56">+IF(OR($E75=$C$5,$E75=$C$6),ROUNDDOWN(AH75/(AI75*AJ75),0),1)</f>
         <v>1</v>
       </c>
       <c r="AL75" s="47">

</xml_diff>